<commit_message>
Aggiornati report-checklist e data
Come comunicato ho corretto in  report-checklist: valorizzata colonna K per applicabilità NO; Inserito Common name del certificato in Nome fornitore;
Rimosso test non applicabile in data.json.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#INFOMATICXX/infomatic.it/Demat190/1.5/report-checklist.xlsx
+++ b/GATEWAY/A1#111#INFOMATICXX/infomatic.it/Demat190/1.5/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Demat\certificati\Accredito\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B946C46C-5724-42D3-9837-964F650D5ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49845F10-B075-4823-9EAB-D010F0DF4689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="531">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1816,9 +1816,6 @@
     <t>c8a6fca997e7ac74942c4c3fbb52f7a8</t>
   </si>
   <si>
-    <t>2025-05-08T20:54:24Z</t>
-  </si>
-  <si>
     <t>2025-05-08T17:43:06Z</t>
   </si>
   <si>
@@ -1988,6 +1985,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.3087f2a2d3caecc6e6809dad81b48ab38cf980a3139055aaa75352fec71d032a.de7cf36008^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Per questo caso di test è richiesta la sola descrizione. Viene simulata l'assenza di connettività. Test autodichiarato.</t>
+  </si>
+  <si>
+    <t>Carmelo</t>
   </si>
 </sst>
 </file>
@@ -2663,6 +2666,9 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2684,9 +2690,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2984,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4137,7 +4140,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H194" sqref="H194"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4149,7 +4152,9 @@
     <col min="5" max="5" width="73.44140625" customWidth="1"/>
     <col min="6" max="9" width="33.21875" customWidth="1"/>
     <col min="10" max="10" width="27.21875" customWidth="1"/>
-    <col min="11" max="18" width="36.44140625" customWidth="1"/>
+    <col min="11" max="11" width="40" customWidth="1"/>
+    <col min="12" max="12" width="53.5546875" customWidth="1"/>
+    <col min="13" max="18" width="36.44140625" customWidth="1"/>
     <col min="19" max="19" width="27.21875" customWidth="1"/>
     <col min="20" max="20" width="33.21875" customWidth="1"/>
     <col min="21" max="21" width="36.44140625" customWidth="1"/>
@@ -4179,12 +4184,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72" t="s">
+        <v>530</v>
+      </c>
+      <c r="D2" s="71"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -4205,14 +4212,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="78" t="s">
+      <c r="B3" s="74"/>
+      <c r="C3" s="79" t="s">
         <v>437</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="71"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -4233,12 +4240,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="78" t="s">
+      <c r="A4" s="75"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="79" t="s">
         <v>438</v>
       </c>
-      <c r="D4" s="70"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -4260,12 +4267,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="76"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="78" t="s">
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="79" t="s">
         <v>439</v>
       </c>
-      <c r="D5" s="70"/>
+      <c r="D5" s="71"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -4286,8 +4293,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67"/>
-      <c r="B6" s="68"/>
+      <c r="A6" s="68"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5271,19 +5278,19 @@
       <c r="E31" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="F31" s="57">
-        <v>45785</v>
-      </c>
-      <c r="G31" s="57" t="s">
-        <v>472</v>
-      </c>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
       <c r="H31" s="57"/>
       <c r="I31" s="58"/>
       <c r="J31" s="59" t="s">
         <v>232</v>
       </c>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
+      <c r="K31" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="L31" s="59" t="s">
+        <v>529</v>
+      </c>
       <c r="M31" s="59" t="s">
         <v>64</v>
       </c>
@@ -5306,9 +5313,7 @@
         <v>444</v>
       </c>
       <c r="T31" s="59"/>
-      <c r="U31" s="60" t="s">
-        <v>64</v>
-      </c>
+      <c r="U31" s="60"/>
       <c r="V31" s="61"/>
       <c r="W31" s="59" t="s">
         <v>44</v>
@@ -8583,13 +8588,13 @@
         <v>45785</v>
       </c>
       <c r="G119" s="37" t="s">
+        <v>472</v>
+      </c>
+      <c r="H119" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="H119" s="37" t="s">
+      <c r="I119" s="42" t="s">
         <v>474</v>
-      </c>
-      <c r="I119" s="42" t="s">
-        <v>475</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -8644,13 +8649,13 @@
         <v>45785</v>
       </c>
       <c r="G120" s="37" t="s">
+        <v>475</v>
+      </c>
+      <c r="H120" s="37" t="s">
         <v>476</v>
       </c>
-      <c r="H120" s="37" t="s">
+      <c r="I120" s="42" t="s">
         <v>477</v>
-      </c>
-      <c r="I120" s="42" t="s">
-        <v>478</v>
       </c>
       <c r="J120" s="38" t="s">
         <v>64</v>
@@ -8705,13 +8710,13 @@
         <v>45785</v>
       </c>
       <c r="G121" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="H121" s="37" t="s">
         <v>479</v>
       </c>
-      <c r="H121" s="37" t="s">
+      <c r="I121" s="42" t="s">
         <v>480</v>
-      </c>
-      <c r="I121" s="42" t="s">
-        <v>481</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -8766,13 +8771,13 @@
         <v>45785</v>
       </c>
       <c r="G122" s="37" t="s">
+        <v>481</v>
+      </c>
+      <c r="H122" s="37" t="s">
         <v>482</v>
       </c>
-      <c r="H122" s="37" t="s">
+      <c r="I122" s="42" t="s">
         <v>483</v>
-      </c>
-      <c r="I122" s="42" t="s">
-        <v>484</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -8827,13 +8832,13 @@
         <v>45785</v>
       </c>
       <c r="G123" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="H123" s="37" t="s">
         <v>485</v>
       </c>
-      <c r="H123" s="37" t="s">
+      <c r="I123" s="42" t="s">
         <v>486</v>
-      </c>
-      <c r="I123" s="42" t="s">
-        <v>487</v>
       </c>
       <c r="J123" s="38" t="s">
         <v>64</v>
@@ -8888,13 +8893,13 @@
         <v>45785</v>
       </c>
       <c r="G124" s="37" t="s">
+        <v>487</v>
+      </c>
+      <c r="H124" s="37" t="s">
         <v>488</v>
       </c>
-      <c r="H124" s="37" t="s">
+      <c r="I124" s="42" t="s">
         <v>489</v>
-      </c>
-      <c r="I124" s="42" t="s">
-        <v>490</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -8949,13 +8954,13 @@
         <v>45785</v>
       </c>
       <c r="G125" s="37" t="s">
+        <v>490</v>
+      </c>
+      <c r="H125" s="37" t="s">
         <v>491</v>
       </c>
-      <c r="H125" s="37" t="s">
+      <c r="I125" s="42" t="s">
         <v>492</v>
-      </c>
-      <c r="I125" s="42" t="s">
-        <v>493</v>
       </c>
       <c r="J125" s="38" t="s">
         <v>64</v>
@@ -9010,13 +9015,13 @@
         <v>45785</v>
       </c>
       <c r="G126" s="37" t="s">
+        <v>493</v>
+      </c>
+      <c r="H126" s="37" t="s">
         <v>494</v>
       </c>
-      <c r="H126" s="37" t="s">
+      <c r="I126" s="42" t="s">
         <v>495</v>
-      </c>
-      <c r="I126" s="42" t="s">
-        <v>496</v>
       </c>
       <c r="J126" s="38" t="s">
         <v>64</v>
@@ -9071,13 +9076,13 @@
         <v>45785</v>
       </c>
       <c r="G127" s="37" t="s">
+        <v>496</v>
+      </c>
+      <c r="H127" s="37" t="s">
         <v>497</v>
       </c>
-      <c r="H127" s="37" t="s">
+      <c r="I127" s="42" t="s">
         <v>498</v>
-      </c>
-      <c r="I127" s="42" t="s">
-        <v>499</v>
       </c>
       <c r="J127" s="38" t="s">
         <v>64</v>
@@ -9132,13 +9137,13 @@
         <v>45785</v>
       </c>
       <c r="G128" s="37" t="s">
+        <v>499</v>
+      </c>
+      <c r="H128" s="37" t="s">
         <v>500</v>
       </c>
-      <c r="H128" s="37" t="s">
+      <c r="I128" s="42" t="s">
         <v>501</v>
-      </c>
-      <c r="I128" s="42" t="s">
-        <v>502</v>
       </c>
       <c r="J128" s="38" t="s">
         <v>64</v>
@@ -9193,13 +9198,13 @@
         <v>45785</v>
       </c>
       <c r="G129" s="37" t="s">
+        <v>502</v>
+      </c>
+      <c r="H129" s="37" t="s">
         <v>503</v>
       </c>
-      <c r="H129" s="37" t="s">
+      <c r="I129" s="42" t="s">
         <v>504</v>
-      </c>
-      <c r="I129" s="42" t="s">
-        <v>505</v>
       </c>
       <c r="J129" s="38" t="s">
         <v>64</v>
@@ -9254,13 +9259,13 @@
         <v>45785</v>
       </c>
       <c r="G130" s="37" t="s">
+        <v>505</v>
+      </c>
+      <c r="H130" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="H130" s="37" t="s">
+      <c r="I130" s="42" t="s">
         <v>507</v>
-      </c>
-      <c r="I130" s="42" t="s">
-        <v>508</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -9315,13 +9320,13 @@
         <v>45785</v>
       </c>
       <c r="G131" s="37" t="s">
+        <v>508</v>
+      </c>
+      <c r="H131" s="37" t="s">
         <v>509</v>
       </c>
-      <c r="H131" s="37" t="s">
+      <c r="I131" s="42" t="s">
         <v>510</v>
-      </c>
-      <c r="I131" s="42" t="s">
-        <v>511</v>
       </c>
       <c r="J131" s="38" t="s">
         <v>64</v>
@@ -9376,13 +9381,13 @@
         <v>45785</v>
       </c>
       <c r="G132" s="37" t="s">
+        <v>511</v>
+      </c>
+      <c r="H132" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="H132" s="37" t="s">
+      <c r="I132" s="42" t="s">
         <v>513</v>
-      </c>
-      <c r="I132" s="42" t="s">
-        <v>514</v>
       </c>
       <c r="J132" s="38" t="s">
         <v>64</v>
@@ -9437,13 +9442,13 @@
         <v>45785</v>
       </c>
       <c r="G133" s="37" t="s">
+        <v>514</v>
+      </c>
+      <c r="H133" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="H133" s="37" t="s">
+      <c r="I133" s="42" t="s">
         <v>516</v>
-      </c>
-      <c r="I133" s="42" t="s">
-        <v>517</v>
       </c>
       <c r="J133" s="38" t="s">
         <v>64</v>
@@ -10793,13 +10798,13 @@
         <v>45785</v>
       </c>
       <c r="G169" s="48" t="s">
+        <v>517</v>
+      </c>
+      <c r="H169" s="48" t="s">
         <v>518</v>
       </c>
-      <c r="H169" s="48" t="s">
+      <c r="I169" s="49" t="s">
         <v>519</v>
-      </c>
-      <c r="I169" s="49" t="s">
-        <v>520</v>
       </c>
       <c r="J169" s="50" t="s">
         <v>64</v>
@@ -10842,13 +10847,13 @@
         <v>45785</v>
       </c>
       <c r="G170" s="48" t="s">
+        <v>520</v>
+      </c>
+      <c r="H170" s="48" t="s">
         <v>521</v>
       </c>
-      <c r="H170" s="48" t="s">
+      <c r="I170" s="49" t="s">
         <v>522</v>
-      </c>
-      <c r="I170" s="49" t="s">
-        <v>523</v>
       </c>
       <c r="J170" s="50" t="s">
         <v>64</v>
@@ -11261,13 +11266,13 @@
         <v>45785</v>
       </c>
       <c r="G181" s="35" t="s">
+        <v>523</v>
+      </c>
+      <c r="H181" s="35" t="s">
         <v>524</v>
       </c>
-      <c r="H181" s="35" t="s">
+      <c r="I181" s="35" t="s">
         <v>525</v>
-      </c>
-      <c r="I181" s="35" t="s">
-        <v>526</v>
       </c>
       <c r="J181" s="38" t="s">
         <v>64</v>
@@ -11544,13 +11549,13 @@
         <v>45785</v>
       </c>
       <c r="G188" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="H188" s="35" t="s">
         <v>527</v>
       </c>
-      <c r="H188" s="35" t="s">
+      <c r="I188" s="35" t="s">
         <v>528</v>
-      </c>
-      <c r="I188" s="35" t="s">
-        <v>529</v>
       </c>
       <c r="J188" s="38" t="s">
         <v>64</v>
@@ -11774,7 +11779,7 @@
       <c r="W194" s="9"/>
     </row>
     <row r="195" spans="6:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F195" s="79"/>
+      <c r="F195" s="67"/>
       <c r="G195" s="6"/>
       <c r="H195" s="6"/>
       <c r="I195" s="6"/>
@@ -18100,15 +18105,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18370,27 +18372,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18415,9 +18411,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>